<commit_message>
refactor tab50 report for consistency and add xlsx to tab 50
</commit_message>
<xml_diff>
--- a/backend/reports/xlsx/Tab_50_rpt_PF_NetRecoverySummaryByQuarter.xlsx
+++ b/backend/reports/xlsx/Tab_50_rpt_PF_NetRecoverySummaryByQuarter.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/robrien/work/gdx-agreements-tracker/backend/reports/xlsx/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{989B08D1-04B0-9749-8564-C8E7373850CC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC34032B-0AEA-564E-A7A1-6D25BEB16419}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="12080" yWindow="-21100" windowWidth="28040" windowHeight="17420" xr2:uid="{FB9893AD-F19A-BB4E-A83D-FCCFB21F8723}"/>
+    <workbookView xWindow="380" yWindow="-18720" windowWidth="28040" windowHeight="17420" xr2:uid="{FB9893AD-F19A-BB4E-A83D-FCCFB21F8723}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>

</xml_diff>

<commit_message>
fix format on xls/doc & missing totals column
</commit_message>
<xml_diff>
--- a/backend/reports/xlsx/Tab_50_rpt_PF_NetRecoverySummaryByQuarter.xlsx
+++ b/backend/reports/xlsx/Tab_50_rpt_PF_NetRecoverySummaryByQuarter.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/robrien/work/gdx-agreements-tracker/backend/reports/xlsx/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC34032B-0AEA-564E-A7A1-6D25BEB16419}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A1C3EE0-1B44-3149-B6CD-579C940136C2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="380" yWindow="-18720" windowWidth="28040" windowHeight="17420" xr2:uid="{FB9893AD-F19A-BB4E-A83D-FCCFB21F8723}"/>
+    <workbookView xWindow="-14280" yWindow="-21100" windowWidth="51200" windowHeight="21100" xr2:uid="{FB9893AD-F19A-BB4E-A83D-FCCFB21F8723}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="42">
   <si>
     <t>{$r1.portfolio_name}</t>
   </si>
@@ -44,15 +44,6 @@
     <t>TOTAL:</t>
   </si>
   <si>
-    <t>{#r = d.report[i]}</t>
-  </si>
-  <si>
-    <t>{#r1= d.report[i+1]}</t>
-  </si>
-  <si>
-    <t>{#t = d.report_totals[i]}</t>
-  </si>
-  <si>
     <t>Total Recoveries For Projects</t>
   </si>
   <si>
@@ -152,14 +143,35 @@
     <t>{$t.totals_q4_net}</t>
   </si>
   <si>
-    <t xml:space="preserve">        Net Recovery Summary By Quarter for Fiscal Year {d.report_totals[0].fiscal_year}</t>
+    <t>{$r.portfolio_name}</t>
+  </si>
+  <si>
+    <t>{#r=d.report[i]}</t>
+  </si>
+  <si>
+    <t>{#r1=d.report[i+1]}</t>
+  </si>
+  <si>
+    <t>{#t=d.report_totals[i]}</t>
+  </si>
+  <si>
+    <t>{#fy=d.fiscal}</t>
+  </si>
+  <si>
+    <t>{#date=d.date}</t>
+  </si>
+  <si>
+    <t>Net Recovery Summary By Quarter for Fiscal Year {$fy}</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00"/>
+  </numFmts>
+  <fonts count="8">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -191,6 +203,12 @@
     </font>
     <font>
       <sz val="18"/>
+      <color theme="0"/>
+      <name val="BCSans-Regular"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="8.5"/>
       <name val="BCSans-Regular"/>
     </font>
   </fonts>
@@ -209,7 +227,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFC5DAF1"/>
+        <fgColor rgb="FF003365"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -289,53 +307,51 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
+    <xf numFmtId="4" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="4" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="4" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right" vertical="center" indent="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right" vertical="center" indent="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right" vertical="center" indent="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="4" fontId="7" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="7" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -345,6 +361,7 @@
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
+      <color rgb="FF003365"/>
       <color rgb="FFC5DAF1"/>
     </mruColors>
   </colors>
@@ -369,17 +386,17 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>795655</xdr:colOff>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>32837</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>719455</xdr:rowOff>
+      <xdr:rowOff>680356</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="image1.jpeg" descr="Logo, company name&#10;&#10;Description automatically generated">
+        <xdr:cNvPr id="4" name="Graphic 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5B3FA340-3BA5-3518-39AF-972CEFDE23A6}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CD3FB7DC-2494-89FE-0AC0-2E0678523FE8}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -388,7 +405,13 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+          <a:extLst>
+            <a:ext uri="{96DAC541-7B7A-43D3-8B79-37D633B846F1}">
+              <asvg:svgBlip xmlns:asvg="http://schemas.microsoft.com/office/drawing/2016/SVG/main" r:embed="rId2"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -396,7 +419,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="0" y="0"/>
-          <a:ext cx="795655" cy="719455"/>
+          <a:ext cx="2412174" cy="680356"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -705,188 +728,206 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0F20F7FF-D6FB-0145-BC76-92F810195548}">
-  <dimension ref="A1:L10"/>
+  <dimension ref="A1:L11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+    <sheetView tabSelected="1" zoomScale="157" zoomScaleNormal="157" workbookViewId="0">
+      <selection sqref="A1:L1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <cols>
+    <col min="1" max="1" width="31.1640625" customWidth="1"/>
+    <col min="2" max="2" width="22.83203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="20.1640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.33203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="17" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="15.33203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="17" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="15.33203125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="17" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="15.33203125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:12" s="1" customFormat="1" ht="57" customHeight="1" thickBot="1">
-      <c r="A1" s="16" t="s">
+      <c r="A1" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="B1" s="3"/>
+      <c r="C1" s="3"/>
+      <c r="D1" s="3"/>
+      <c r="E1" s="3"/>
+      <c r="F1" s="3"/>
+      <c r="G1" s="3"/>
+      <c r="H1" s="3"/>
+      <c r="I1" s="3"/>
+      <c r="J1" s="3"/>
+      <c r="K1" s="3"/>
+      <c r="L1" s="3"/>
+    </row>
+    <row r="2" spans="1:12" s="1" customFormat="1" ht="20" thickBot="1">
+      <c r="A2" s="4"/>
+      <c r="B2" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="D2" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="E2" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="F2" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="G2" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="H2" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="I2" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="J2" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="K2" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="L2" s="6" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" s="2" customFormat="1" ht="20" thickBot="1">
+      <c r="A3" s="14" t="s">
+        <v>35</v>
+      </c>
+      <c r="B3" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="C3" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="D3" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="E3" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="F3" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="G3" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="H3" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="I3" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="J3" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="K3" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="L3" s="9" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" s="2" customFormat="1" ht="20" thickBot="1">
+      <c r="A4" s="15" t="s">
+        <v>0</v>
+      </c>
+      <c r="B4" s="7"/>
+      <c r="C4" s="8"/>
+      <c r="D4" s="9"/>
+      <c r="E4" s="8"/>
+      <c r="F4" s="9"/>
+      <c r="G4" s="8"/>
+      <c r="H4" s="9"/>
+      <c r="I4" s="8"/>
+      <c r="J4" s="9"/>
+      <c r="K4" s="8"/>
+      <c r="L4" s="9"/>
+    </row>
+    <row r="5" spans="1:12" s="1" customFormat="1" ht="20" thickBot="1">
+      <c r="A5" s="13" t="s">
+        <v>1</v>
+      </c>
+      <c r="B5" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="C5" s="11" t="s">
+        <v>25</v>
+      </c>
+      <c r="D5" s="12" t="s">
+        <v>26</v>
+      </c>
+      <c r="E5" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="F5" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="G5" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="H5" s="12" t="s">
+        <v>30</v>
+      </c>
+      <c r="I5" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="J5" s="12" t="s">
+        <v>32</v>
+      </c>
+      <c r="K5" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="L5" s="12" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12">
+      <c r="A7" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12">
+      <c r="A8" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12">
+      <c r="A9" t="s">
         <v>38</v>
       </c>
-      <c r="B1" s="16"/>
-      <c r="C1" s="16"/>
-      <c r="D1" s="16"/>
-      <c r="E1" s="16"/>
-      <c r="F1" s="16"/>
-      <c r="G1" s="16"/>
-      <c r="H1" s="16"/>
-      <c r="I1" s="16"/>
-      <c r="J1" s="16"/>
-      <c r="K1" s="16"/>
-      <c r="L1" s="16"/>
     </row>
-    <row r="2" spans="1:12" s="1" customFormat="1" ht="189" customHeight="1" thickBot="1">
-      <c r="A2" s="2"/>
-      <c r="B2" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="D2" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="E2" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="F2" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="G2" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="H2" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="I2" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="J2" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="K2" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="L2" s="4" t="s">
-        <v>14</v>
+    <row r="10" spans="1:12">
+      <c r="A10" t="s">
+        <v>39</v>
       </c>
     </row>
-    <row r="3" spans="1:12" s="1" customFormat="1" ht="49" thickBot="1">
-      <c r="A3" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="B3" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="C3" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="D3" s="8" t="s">
-        <v>18</v>
-      </c>
-      <c r="E3" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="F3" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="G3" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="H3" s="8" t="s">
-        <v>22</v>
-      </c>
-      <c r="I3" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="J3" s="8" t="s">
-        <v>24</v>
-      </c>
-      <c r="K3" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="L3" s="8" t="s">
-        <v>26</v>
+    <row r="11" spans="1:12">
+      <c r="A11" t="s">
+        <v>40</v>
       </c>
     </row>
-    <row r="4" spans="1:12" s="1" customFormat="1" ht="33" thickBot="1">
-      <c r="A4" s="9" t="s">
-        <v>0</v>
-      </c>
-      <c r="B4" s="7"/>
-      <c r="C4" s="7"/>
-      <c r="D4" s="8"/>
-      <c r="E4" s="7"/>
-      <c r="F4" s="8"/>
-      <c r="G4" s="7"/>
-      <c r="H4" s="8"/>
-      <c r="I4" s="7"/>
-      <c r="J4" s="8"/>
-      <c r="K4" s="7"/>
-      <c r="L4" s="8"/>
-    </row>
-    <row r="5" spans="1:12" s="1" customFormat="1" ht="43" thickBot="1">
-      <c r="A5" s="10" t="s">
-        <v>1</v>
-      </c>
-      <c r="B5" s="11" t="s">
-        <v>27</v>
-      </c>
-      <c r="C5" s="12" t="s">
-        <v>28</v>
-      </c>
-      <c r="D5" s="13" t="s">
-        <v>29</v>
-      </c>
-      <c r="E5" s="12" t="s">
-        <v>30</v>
-      </c>
-      <c r="F5" s="13" t="s">
-        <v>31</v>
-      </c>
-      <c r="G5" s="12" t="s">
-        <v>32</v>
-      </c>
-      <c r="H5" s="13" t="s">
-        <v>33</v>
-      </c>
-      <c r="I5" s="12" t="s">
-        <v>34</v>
-      </c>
-      <c r="J5" s="13" t="s">
-        <v>35</v>
-      </c>
-      <c r="K5" s="12" t="s">
-        <v>36</v>
-      </c>
-      <c r="L5" s="13" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="6" spans="1:12" s="1" customFormat="1" ht="19">
-      <c r="A6" s="14"/>
-    </row>
-    <row r="7" spans="1:12" s="1" customFormat="1" ht="19">
-      <c r="A7" s="15" t="s">
-        <v>2</v>
-      </c>
-      <c r="B7" s="15"/>
-    </row>
-    <row r="8" spans="1:12" s="1" customFormat="1" ht="19">
-      <c r="A8" s="15" t="s">
-        <v>3</v>
-      </c>
-      <c r="B8" s="15"/>
-    </row>
-    <row r="9" spans="1:12" s="1" customFormat="1" ht="19">
-      <c r="A9" s="15" t="s">
-        <v>4</v>
-      </c>
-      <c r="B9" s="15"/>
-    </row>
-    <row r="10" spans="1:12" s="1" customFormat="1" ht="19"/>
   </sheetData>
-  <mergeCells count="4">
+  <mergeCells count="1">
     <mergeCell ref="A1:L1"/>
-    <mergeCell ref="A7:B7"/>
-    <mergeCell ref="A8:B8"/>
-    <mergeCell ref="A9:B9"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="5" orientation="landscape" horizontalDpi="0" verticalDpi="0"/>
+  <headerFooter>
+    <oddFooter>&amp;Lrpt_PF_NetRecoverySummaryByQuarter&amp;C&amp;P of &amp;N&amp;R{$date}</oddFooter>
+  </headerFooter>
   <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
refactor controller for reports to be more generic
* the model will handle the data manipulations
* the controller will simply call the model's method depending on which
  attribute we want to orgainize the results by, e.g. fiscal year, or
  portfolio name.
</commit_message>
<xml_diff>
--- a/backend/reports/xlsx/Tab_50_rpt_PF_NetRecoverySummaryByQuarter.xlsx
+++ b/backend/reports/xlsx/Tab_50_rpt_PF_NetRecoverySummaryByQuarter.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10514"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10611"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/robrien/work/gdx-agreements-tracker/backend/reports/xlsx/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A1C3EE0-1B44-3149-B6CD-579C940136C2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{24E9EC59-9ECB-1149-8C0C-687A8EB0C6FC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-14280" yWindow="-21100" windowWidth="51200" windowHeight="21100" xr2:uid="{FB9893AD-F19A-BB4E-A83D-FCCFB21F8723}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="43">
   <si>
     <t>{$r1.portfolio_name}</t>
   </si>
@@ -162,6 +162,9 @@
   </si>
   <si>
     <t>Net Recovery Summary By Quarter for Fiscal Year {$fy}</t>
+  </si>
+  <si>
+    <t>Portfolios</t>
   </si>
 </sst>
 </file>
@@ -171,7 +174,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00"/>
   </numFmts>
-  <fonts count="8">
+  <fonts count="7">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -181,10 +184,6 @@
     </font>
     <font>
       <sz val="12"/>
-      <name val="BCSans-Regular"/>
-    </font>
-    <font>
-      <sz val="9"/>
       <name val="BCSans-Regular"/>
     </font>
     <font>
@@ -307,51 +306,54 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="4" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="4" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="4" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="4" fontId="4" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="4" fontId="3" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="4" fontId="4" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="4" fontId="3" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="right" vertical="center" indent="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="right" vertical="center" indent="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="right" vertical="center" indent="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" indent="1"/>
     </xf>
-    <xf numFmtId="4" fontId="7" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="4" fontId="6" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="4" fontId="7" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="4" fontId="6" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -731,7 +733,7 @@
   <dimension ref="A1:L11"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="157" zoomScaleNormal="157" workbookViewId="0">
-      <selection sqref="A1:L1"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -751,146 +753,148 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" s="1" customFormat="1" ht="57" customHeight="1" thickBot="1">
-      <c r="A1" s="3" t="s">
+      <c r="A1" s="15" t="s">
         <v>41</v>
       </c>
-      <c r="B1" s="3"/>
-      <c r="C1" s="3"/>
-      <c r="D1" s="3"/>
-      <c r="E1" s="3"/>
-      <c r="F1" s="3"/>
-      <c r="G1" s="3"/>
-      <c r="H1" s="3"/>
-      <c r="I1" s="3"/>
-      <c r="J1" s="3"/>
-      <c r="K1" s="3"/>
-      <c r="L1" s="3"/>
+      <c r="B1" s="14"/>
+      <c r="C1" s="14"/>
+      <c r="D1" s="14"/>
+      <c r="E1" s="14"/>
+      <c r="F1" s="14"/>
+      <c r="G1" s="14"/>
+      <c r="H1" s="14"/>
+      <c r="I1" s="14"/>
+      <c r="J1" s="14"/>
+      <c r="K1" s="14"/>
+      <c r="L1" s="14"/>
     </row>
     <row r="2" spans="1:12" s="1" customFormat="1" ht="20" thickBot="1">
-      <c r="A2" s="4"/>
-      <c r="B2" s="5" t="s">
+      <c r="A2" s="16" t="s">
+        <v>42</v>
+      </c>
+      <c r="B2" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="5" t="s">
+      <c r="C2" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="6" t="s">
+      <c r="D2" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="E2" s="5" t="s">
+      <c r="E2" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="F2" s="6" t="s">
+      <c r="F2" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="G2" s="5" t="s">
+      <c r="G2" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="H2" s="6" t="s">
+      <c r="H2" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="I2" s="5" t="s">
+      <c r="I2" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="J2" s="6" t="s">
+      <c r="J2" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="K2" s="5" t="s">
+      <c r="K2" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="L2" s="6" t="s">
+      <c r="L2" s="4" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="3" spans="1:12" s="2" customFormat="1" ht="20" thickBot="1">
-      <c r="A3" s="14" t="s">
+      <c r="A3" s="12" t="s">
         <v>35</v>
       </c>
-      <c r="B3" s="7" t="s">
+      <c r="B3" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="C3" s="8" t="s">
+      <c r="C3" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="D3" s="9" t="s">
+      <c r="D3" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="E3" s="8" t="s">
+      <c r="E3" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="F3" s="9" t="s">
+      <c r="F3" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="G3" s="8" t="s">
+      <c r="G3" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="H3" s="9" t="s">
+      <c r="H3" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="I3" s="8" t="s">
+      <c r="I3" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="J3" s="9" t="s">
+      <c r="J3" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="K3" s="8" t="s">
+      <c r="K3" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="L3" s="9" t="s">
+      <c r="L3" s="7" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="4" spans="1:12" s="2" customFormat="1" ht="20" thickBot="1">
-      <c r="A4" s="15" t="s">
+      <c r="A4" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="B4" s="7"/>
-      <c r="C4" s="8"/>
-      <c r="D4" s="9"/>
-      <c r="E4" s="8"/>
-      <c r="F4" s="9"/>
-      <c r="G4" s="8"/>
-      <c r="H4" s="9"/>
-      <c r="I4" s="8"/>
-      <c r="J4" s="9"/>
-      <c r="K4" s="8"/>
-      <c r="L4" s="9"/>
+      <c r="B4" s="5"/>
+      <c r="C4" s="6"/>
+      <c r="D4" s="7"/>
+      <c r="E4" s="6"/>
+      <c r="F4" s="7"/>
+      <c r="G4" s="6"/>
+      <c r="H4" s="7"/>
+      <c r="I4" s="6"/>
+      <c r="J4" s="7"/>
+      <c r="K4" s="6"/>
+      <c r="L4" s="7"/>
     </row>
     <row r="5" spans="1:12" s="1" customFormat="1" ht="20" thickBot="1">
-      <c r="A5" s="13" t="s">
+      <c r="A5" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="B5" s="10" t="s">
+      <c r="B5" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="C5" s="11" t="s">
+      <c r="C5" s="9" t="s">
         <v>25</v>
       </c>
-      <c r="D5" s="12" t="s">
+      <c r="D5" s="10" t="s">
         <v>26</v>
       </c>
-      <c r="E5" s="11" t="s">
+      <c r="E5" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="F5" s="12" t="s">
+      <c r="F5" s="10" t="s">
         <v>28</v>
       </c>
-      <c r="G5" s="11" t="s">
+      <c r="G5" s="9" t="s">
         <v>29</v>
       </c>
-      <c r="H5" s="12" t="s">
+      <c r="H5" s="10" t="s">
         <v>30</v>
       </c>
-      <c r="I5" s="11" t="s">
+      <c r="I5" s="9" t="s">
         <v>31</v>
       </c>
-      <c r="J5" s="12" t="s">
+      <c r="J5" s="10" t="s">
         <v>32</v>
       </c>
-      <c r="K5" s="11" t="s">
+      <c r="K5" s="9" t="s">
         <v>33</v>
       </c>
-      <c r="L5" s="12" t="s">
+      <c r="L5" s="10" t="s">
         <v>34</v>
       </c>
     </row>

</xml_diff>